<commit_message>
add folder for algo2_files
</commit_message>
<xml_diff>
--- a/docs/compare_Algo1_outputs.xlsx
+++ b/docs/compare_Algo1_outputs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="275">
   <si>
     <t>Ariel_University</t>
   </si>
@@ -825,13 +825,22 @@
     <t>SAME</t>
   </si>
   <si>
-    <t>DIFF</t>
-  </si>
-  <si>
     <t>my_signal</t>
   </si>
   <si>
     <t>boaz_signal</t>
+  </si>
+  <si>
+    <t>Diff Lon</t>
+  </si>
+  <si>
+    <t>Diff Lat</t>
+  </si>
+  <si>
+    <t>Diff Alt</t>
+  </si>
+  <si>
+    <t>Same?</t>
   </si>
 </sst>
 </file>
@@ -9878,30 +9887,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J142"/>
+  <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="7" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>261</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>262</v>
@@ -9913,7 +9923,7 @@
         <v>267</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>265</v>
@@ -9925,10 +9935,19 @@
         <v>266</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>57</v>
       </c>
@@ -9956,8 +9975,20 @@
       <c r="I2" s="12">
         <v>685</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <f>ABS(E2-I2)</f>
+        <v>6898056423384105</v>
+      </c>
+      <c r="L2">
+        <f>ABS(D2-G2)</f>
+        <v>3210375586148489</v>
+      </c>
+      <c r="M2">
+        <f>ABS(C2-H2)</f>
+        <v>3520917794137017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>115</v>
       </c>
@@ -9988,8 +10019,20 @@
       <c r="J3" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="12">
+        <f t="shared" ref="K3:K66" si="0">ABS(E3-I3)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="12">
+        <f t="shared" ref="L3:L66" si="1">ABS(D3-G3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="12">
+        <f t="shared" ref="M3:M66" si="2">ABS(C3-H3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -10020,8 +10063,20 @@
       <c r="J4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>196</v>
       </c>
@@ -10052,8 +10107,20 @@
       <c r="J5" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>31</v>
       </c>
@@ -10081,8 +10148,20 @@
       <c r="I6" s="12">
         <v>689</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="12">
+        <f t="shared" si="0"/>
+        <v>6904225175125211</v>
+      </c>
+      <c r="L6" s="12">
+        <f t="shared" si="1"/>
+        <v>3.2104754652700356E+16</v>
+      </c>
+      <c r="M6" s="12">
+        <f t="shared" si="2"/>
+        <v>3521027571678466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>118</v>
       </c>
@@ -10113,8 +10192,20 @@
       <c r="J7" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>210</v>
       </c>
@@ -10145,8 +10236,20 @@
       <c r="J8" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>189</v>
       </c>
@@ -10177,8 +10280,20 @@
       <c r="J9" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>75</v>
       </c>
@@ -10206,8 +10321,20 @@
       <c r="I10" s="12">
         <v>686</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="12">
+        <f t="shared" si="0"/>
+        <v>6867540774908114</v>
+      </c>
+      <c r="L10" s="12">
+        <f t="shared" si="1"/>
+        <v>3210312829142143</v>
+      </c>
+      <c r="M10" s="12">
+        <f t="shared" si="2"/>
+        <v>3.168792464447412E+16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>79</v>
       </c>
@@ -10238,8 +10365,20 @@
       <c r="J11" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>120</v>
       </c>
@@ -10270,8 +10409,20 @@
       <c r="J12" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>161</v>
       </c>
@@ -10302,8 +10453,20 @@
       <c r="J13" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>122</v>
       </c>
@@ -10331,8 +10494,20 @@
       <c r="I14" s="13">
         <v>6983196084604080</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="12">
+        <f t="shared" si="0"/>
+        <v>33911675808170</v>
+      </c>
+      <c r="L14" s="12">
+        <f t="shared" si="1"/>
+        <v>18085086420</v>
+      </c>
+      <c r="M14" s="12">
+        <f t="shared" si="2"/>
+        <v>3.16889705052685E+16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>178</v>
       </c>
@@ -10363,8 +10538,20 @@
       <c r="J15" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>27</v>
       </c>
@@ -10392,8 +10579,20 @@
       <c r="I16" s="13">
         <v>6939879864159310</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="12">
+        <f t="shared" si="0"/>
+        <v>57692278735050</v>
+      </c>
+      <c r="L16" s="12">
+        <f t="shared" si="1"/>
+        <v>10391219130</v>
+      </c>
+      <c r="M16" s="12">
+        <f t="shared" si="2"/>
+        <v>3.169004278398938E+16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>104</v>
       </c>
@@ -10424,8 +10623,20 @@
       <c r="J17" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>106</v>
       </c>
@@ -10453,8 +10664,20 @@
       <c r="I18" s="12">
         <v>690</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="12">
+        <f t="shared" si="0"/>
+        <v>6898094360267540</v>
+      </c>
+      <c r="L18" s="12">
+        <f t="shared" si="1"/>
+        <v>3.2102195347883168E+16</v>
+      </c>
+      <c r="M18" s="12">
+        <f t="shared" si="2"/>
+        <v>3.1688470416939E+16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>193</v>
       </c>
@@ -10485,8 +10708,20 @@
       <c r="J19" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>184</v>
       </c>
@@ -10517,8 +10752,20 @@
       <c r="J20" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>84</v>
       </c>
@@ -10549,8 +10796,20 @@
       <c r="J21" s="5" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="12">
+        <f t="shared" si="0"/>
+        <v>6190649097348135</v>
+      </c>
+      <c r="L21" s="12">
+        <f t="shared" si="1"/>
+        <v>2.8892902641280312E+16</v>
+      </c>
+      <c r="M21" s="12">
+        <f t="shared" si="2"/>
+        <v>49387348880</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>123</v>
       </c>
@@ -10581,8 +10840,20 @@
       <c r="J22" s="6" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="12">
+        <f t="shared" si="0"/>
+        <v>1072054108060</v>
+      </c>
+      <c r="L22" s="12">
+        <f t="shared" si="1"/>
+        <v>8595916810</v>
+      </c>
+      <c r="M22" s="12">
+        <f t="shared" si="2"/>
+        <v>3.16888913846129E+16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>155</v>
       </c>
@@ -10613,8 +10884,20 @@
       <c r="J23" s="7" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="12">
+        <f t="shared" si="0"/>
+        <v>29146010363500</v>
+      </c>
+      <c r="L23" s="12">
+        <f t="shared" si="1"/>
+        <v>1631677800</v>
+      </c>
+      <c r="M23" s="12">
+        <f t="shared" si="2"/>
+        <v>3.168872687392788E+16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>85</v>
       </c>
@@ -10645,8 +10928,20 @@
       <c r="J24" s="8" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>102</v>
       </c>
@@ -10677,8 +10972,20 @@
       <c r="J25" s="10" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>55</v>
       </c>
@@ -10706,8 +11013,20 @@
       <c r="I26" s="13">
         <v>6962530309269260</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="12">
+        <f t="shared" si="0"/>
+        <v>64473885884470</v>
+      </c>
+      <c r="L26" s="12">
+        <f t="shared" si="1"/>
+        <v>6383215550</v>
+      </c>
+      <c r="M26" s="12">
+        <f t="shared" si="2"/>
+        <v>3.1689100853069648E+16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>229</v>
       </c>
@@ -10738,8 +11057,20 @@
       <c r="J27" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>112</v>
       </c>
@@ -10767,8 +11098,20 @@
       <c r="I28" s="13">
         <v>6908556103218320</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="12">
+        <f t="shared" si="0"/>
+        <v>7642089360030</v>
+      </c>
+      <c r="L28" s="12">
+        <f t="shared" si="1"/>
+        <v>2.889227470538774E+16</v>
+      </c>
+      <c r="M28" s="12">
+        <f t="shared" si="2"/>
+        <v>3.1688518116100112E+16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>236</v>
       </c>
@@ -10799,8 +11142,20 @@
       <c r="J29" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>42</v>
       </c>
@@ -10831,8 +11186,20 @@
       <c r="J30" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>6</v>
       </c>
@@ -10863,8 +11230,20 @@
       <c r="J31" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>113</v>
       </c>
@@ -10895,8 +11274,20 @@
       <c r="J32" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>237</v>
       </c>
@@ -10927,8 +11318,20 @@
       <c r="J33" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>26</v>
       </c>
@@ -10956,8 +11359,20 @@
       <c r="I34" s="13">
         <v>694780305912792</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="12">
+        <f t="shared" si="0"/>
+        <v>6187407279511468</v>
+      </c>
+      <c r="L34" s="12">
+        <f t="shared" si="1"/>
+        <v>31194512540</v>
+      </c>
+      <c r="M34" s="12">
+        <f t="shared" si="2"/>
+        <v>76758899760</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>25</v>
       </c>
@@ -10985,8 +11400,20 @@
       <c r="I35" s="13">
         <v>6900233910129260</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="12">
+        <f t="shared" si="0"/>
+        <v>18046324705000</v>
+      </c>
+      <c r="L35" s="12">
+        <f t="shared" si="1"/>
+        <v>2.8894382434324088E+16</v>
+      </c>
+      <c r="M35" s="12">
+        <f t="shared" si="2"/>
+        <v>3.168980139599748E+16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>1</v>
       </c>
@@ -11017,8 +11444,20 @@
       <c r="J36" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>13</v>
       </c>
@@ -11046,8 +11485,20 @@
       <c r="I37" s="13">
         <v>692796460176991</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="12">
+        <f t="shared" si="0"/>
+        <v>6228654769489339</v>
+      </c>
+      <c r="L37" s="12">
+        <f t="shared" si="1"/>
+        <v>3006518280</v>
+      </c>
+      <c r="M37" s="12">
+        <f t="shared" si="2"/>
+        <v>5777306770</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>127</v>
       </c>
@@ -11075,8 +11526,20 @@
       <c r="I38" s="12">
         <v>693</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="12">
+        <f t="shared" si="0"/>
+        <v>7058336904682957</v>
+      </c>
+      <c r="L38" s="12">
+        <f t="shared" si="1"/>
+        <v>3210279128734674</v>
+      </c>
+      <c r="M38" s="12">
+        <f t="shared" si="2"/>
+        <v>3520987524186994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>163</v>
       </c>
@@ -11107,8 +11570,20 @@
       <c r="J39" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>205</v>
       </c>
@@ -11139,8 +11614,20 @@
       <c r="J40" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>202</v>
       </c>
@@ -11171,8 +11658,20 @@
       <c r="J41" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L41" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="12">
+        <f t="shared" si="2"/>
+        <v>3.168891499044276E+16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>14</v>
       </c>
@@ -11203,8 +11702,20 @@
       <c r="J42" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="12">
+        <f t="shared" si="0"/>
+        <v>22280098167000</v>
+      </c>
+      <c r="L42" s="12">
+        <f t="shared" si="1"/>
+        <v>4445107620</v>
+      </c>
+      <c r="M42" s="12">
+        <f t="shared" si="2"/>
+        <v>22569641040</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>66</v>
       </c>
@@ -11232,8 +11743,20 @@
       <c r="I43" s="13">
         <v>6986908557589470</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="12">
+        <f t="shared" si="0"/>
+        <v>131548620857400</v>
+      </c>
+      <c r="L43" s="12">
+        <f t="shared" si="1"/>
+        <v>2.889317181813516E+16</v>
+      </c>
+      <c r="M43" s="12">
+        <f t="shared" si="2"/>
+        <v>109433642790</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>200</v>
       </c>
@@ -11264,8 +11787,20 @@
       <c r="J44" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>149</v>
       </c>
@@ -11296,8 +11831,20 @@
       <c r="J45" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>8</v>
       </c>
@@ -11328,8 +11875,20 @@
       <c r="J46" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>28</v>
       </c>
@@ -11360,8 +11919,20 @@
       <c r="J47" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L47" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>131</v>
       </c>
@@ -11389,8 +11960,20 @@
       <c r="I48" s="13">
         <v>7026309578676630</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="12">
+        <f t="shared" si="0"/>
+        <v>10625472399680</v>
+      </c>
+      <c r="L48" s="12">
+        <f t="shared" si="1"/>
+        <v>8222567370</v>
+      </c>
+      <c r="M48" s="12">
+        <f t="shared" si="2"/>
+        <v>3.1689076808156592E+16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>128</v>
       </c>
@@ -11418,8 +12001,20 @@
       <c r="I49" s="13">
         <v>6991933277572540</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="12">
+        <f t="shared" si="0"/>
+        <v>66403627111110</v>
+      </c>
+      <c r="L49" s="12">
+        <f t="shared" si="1"/>
+        <v>76169214210</v>
+      </c>
+      <c r="M49" s="12">
+        <f t="shared" si="2"/>
+        <v>3.168940515805096E+16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>97</v>
       </c>
@@ -11447,8 +12042,20 @@
       <c r="I50" s="13">
         <v>6907003681992670</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="12">
+        <f t="shared" si="0"/>
+        <v>6217430432833251</v>
+      </c>
+      <c r="L50" s="12">
+        <f t="shared" si="1"/>
+        <v>2.8892309917035672E+16</v>
+      </c>
+      <c r="M50" s="12">
+        <f t="shared" si="2"/>
+        <v>3168848918220064</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>94</v>
       </c>
@@ -11476,8 +12083,20 @@
       <c r="I51" s="12">
         <v>688</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="12">
+        <f t="shared" si="0"/>
+        <v>6889962870267182</v>
+      </c>
+      <c r="L51" s="12">
+        <f t="shared" si="1"/>
+        <v>3210262685085658</v>
+      </c>
+      <c r="M51" s="12">
+        <f t="shared" si="2"/>
+        <v>3520890677223591</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>51</v>
       </c>
@@ -11508,8 +12127,20 @@
       <c r="J52" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="12">
+        <f t="shared" si="0"/>
+        <v>6869999999999313</v>
+      </c>
+      <c r="L52" s="12">
+        <f t="shared" si="1"/>
+        <v>2.88936585270144E+16</v>
+      </c>
+      <c r="M52" s="12">
+        <f t="shared" si="2"/>
+        <v>12619500360</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>71</v>
       </c>
@@ -11537,8 +12168,20 @@
       <c r="I53" s="13">
         <v>6981977167515360</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="12">
+        <f t="shared" si="0"/>
+        <v>6981977167514674</v>
+      </c>
+      <c r="L53" s="12">
+        <f t="shared" si="1"/>
+        <v>2.8893369073509192E+16</v>
+      </c>
+      <c r="M53" s="12">
+        <f t="shared" si="2"/>
+        <v>63876928560</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>63</v>
       </c>
@@ -11566,8 +12209,20 @@
       <c r="I54" s="13">
         <v>685700714863043</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54" s="12">
+        <f t="shared" si="0"/>
+        <v>6169659221869027</v>
+      </c>
+      <c r="L54" s="12">
+        <f t="shared" si="1"/>
+        <v>155992759300</v>
+      </c>
+      <c r="M54" s="12">
+        <f t="shared" si="2"/>
+        <v>3586982380</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>226</v>
       </c>
@@ -11598,8 +12253,20 @@
       <c r="J55" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L55" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>81</v>
       </c>
@@ -11627,8 +12294,20 @@
       <c r="I56" s="13">
         <v>6881025051333150</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56" s="12">
+        <f t="shared" si="0"/>
+        <v>6190216836985815</v>
+      </c>
+      <c r="L56" s="12">
+        <f t="shared" si="1"/>
+        <v>568866323600</v>
+      </c>
+      <c r="M56" s="12">
+        <f t="shared" si="2"/>
+        <v>41439557170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>22</v>
       </c>
@@ -11656,8 +12335,20 @@
       <c r="I57" s="13">
         <v>6927648360769120</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57" s="12">
+        <f t="shared" si="0"/>
+        <v>45460775344860</v>
+      </c>
+      <c r="L57" s="12">
+        <f t="shared" si="1"/>
+        <v>2.8894387732335192E+16</v>
+      </c>
+      <c r="M57" s="12">
+        <f t="shared" si="2"/>
+        <v>71646209190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>4</v>
       </c>
@@ -11688,8 +12379,20 @@
       <c r="J58" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L58" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M58" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>52</v>
       </c>
@@ -11717,8 +12420,20 @@
       <c r="I59" s="13">
         <v>6855370355129230</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59" s="12">
+        <f t="shared" si="0"/>
+        <v>9106753679410</v>
+      </c>
+      <c r="L59" s="12">
+        <f t="shared" si="1"/>
+        <v>148963873300</v>
+      </c>
+      <c r="M59" s="12">
+        <f t="shared" si="2"/>
+        <v>3.168824730233846E+16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>147</v>
       </c>
@@ -11749,8 +12464,20 @@
       <c r="J60" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L60" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M60" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>72</v>
       </c>
@@ -11781,8 +12508,20 @@
       <c r="J61" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61" s="12">
+        <f t="shared" si="0"/>
+        <v>6859999999999304</v>
+      </c>
+      <c r="L61" s="12">
+        <f t="shared" si="1"/>
+        <v>16962067090</v>
+      </c>
+      <c r="M61" s="12">
+        <f t="shared" si="2"/>
+        <v>1278472200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
         <v>175</v>
       </c>
@@ -11813,8 +12552,20 @@
       <c r="J62" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L62" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M62" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>129</v>
       </c>
@@ -11845,8 +12596,20 @@
       <c r="J63" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M63" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
         <v>154</v>
       </c>
@@ -11874,8 +12637,20 @@
       <c r="I64" s="13">
         <v>7021428799579670</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64" s="12">
+        <f t="shared" si="0"/>
+        <v>37580236380610</v>
+      </c>
+      <c r="L64" s="12">
+        <f t="shared" si="1"/>
+        <v>2.8892643405430192E+16</v>
+      </c>
+      <c r="M64" s="12">
+        <f t="shared" si="2"/>
+        <v>302566970</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
         <v>132</v>
       </c>
@@ -11903,8 +12678,20 @@
       <c r="I65" s="13">
         <v>697529939046253</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65" s="12">
+        <f t="shared" si="0"/>
+        <v>6339405112030057</v>
+      </c>
+      <c r="L65" s="12">
+        <f t="shared" si="1"/>
+        <v>2.889337377770716E+16</v>
+      </c>
+      <c r="M65" s="12">
+        <f t="shared" si="2"/>
+        <v>3.168903664053234E+16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
         <v>98</v>
       </c>
@@ -11932,8 +12719,20 @@
       <c r="I66" s="13">
         <v>6964616326009580</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66" s="12">
+        <f t="shared" si="0"/>
+        <v>6275043076850161</v>
+      </c>
+      <c r="L66" s="12">
+        <f t="shared" si="1"/>
+        <v>39250928960</v>
+      </c>
+      <c r="M66" s="12">
+        <f t="shared" si="2"/>
+        <v>3168856637991274</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>157</v>
       </c>
@@ -11961,8 +12760,20 @@
       <c r="I67" s="13">
         <v>7072504239181120</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67" s="12">
+        <f t="shared" ref="K67:K130" si="3">ABS(E67-I67)</f>
+        <v>21929429237950</v>
+      </c>
+      <c r="L67" s="12">
+        <f t="shared" ref="L67:L130" si="4">ABS(D67-G67)</f>
+        <v>2.8892950777481992E+16</v>
+      </c>
+      <c r="M67" s="12">
+        <f t="shared" ref="M67:M130" si="5">ABS(C67-H67)</f>
+        <v>3.168871886347942E+16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
         <v>87</v>
       </c>
@@ -11990,8 +12801,20 @@
       <c r="I68" s="13">
         <v>6865066386555650</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68" s="12">
+        <f t="shared" si="3"/>
+        <v>20840484106820</v>
+      </c>
+      <c r="L68" s="12">
+        <f t="shared" si="4"/>
+        <v>2889221883227297</v>
+      </c>
+      <c r="M68" s="12">
+        <f t="shared" si="5"/>
+        <v>184782206800</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
         <v>76</v>
       </c>
@@ -12022,8 +12845,20 @@
       <c r="J69" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L69" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M69" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
         <v>92</v>
       </c>
@@ -12051,8 +12886,20 @@
       <c r="I70" s="12">
         <v>688</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70" s="12">
+        <f t="shared" si="3"/>
+        <v>6889962870267182</v>
+      </c>
+      <c r="L70" s="12">
+        <f t="shared" si="4"/>
+        <v>3210262685085658</v>
+      </c>
+      <c r="M70" s="12">
+        <f t="shared" si="5"/>
+        <v>3520890677223591</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>144</v>
       </c>
@@ -12083,8 +12930,20 @@
       <c r="J71" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L71" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M71" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
         <v>180</v>
       </c>
@@ -12112,8 +12971,20 @@
       <c r="I72" s="13">
         <v>7047471856325680</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72" s="12">
+        <f t="shared" si="3"/>
+        <v>21632303504460</v>
+      </c>
+      <c r="L72" s="12">
+        <f t="shared" si="4"/>
+        <v>2.8892667127056192E+16</v>
+      </c>
+      <c r="M72" s="12">
+        <f t="shared" si="5"/>
+        <v>785519380</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
         <v>170</v>
       </c>
@@ -12144,8 +13015,20 @@
       <c r="J73" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L73" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M73" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
         <v>191</v>
       </c>
@@ -12176,8 +13059,20 @@
       <c r="J74" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L74" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M74" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
         <v>156</v>
       </c>
@@ -12205,8 +13100,20 @@
       <c r="I75" s="13">
         <v>7021428799579670</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K75" s="12">
+        <f t="shared" si="3"/>
+        <v>29146010363500</v>
+      </c>
+      <c r="L75" s="12">
+        <f t="shared" si="4"/>
+        <v>1631677800</v>
+      </c>
+      <c r="M75" s="12">
+        <f t="shared" si="5"/>
+        <v>3.168872687392788E+16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
         <v>168</v>
       </c>
@@ -12237,8 +13144,20 @@
       <c r="J76" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K76" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L76" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M76" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
         <v>235</v>
       </c>
@@ -12269,8 +13188,20 @@
       <c r="J77" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K77" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L77" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M77" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
         <v>233</v>
       </c>
@@ -12301,8 +13232,20 @@
       <c r="J78" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L78" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M78" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
         <v>142</v>
       </c>
@@ -12333,8 +13276,20 @@
       <c r="J79" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L79" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M79" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
         <v>167</v>
       </c>
@@ -12362,8 +13317,20 @@
       <c r="I80" s="13">
         <v>7078478868628160</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80" s="12">
+        <f t="shared" si="3"/>
+        <v>25542749846120</v>
+      </c>
+      <c r="L80" s="12">
+        <f t="shared" si="4"/>
+        <v>2.88926590141864E+16</v>
+      </c>
+      <c r="M80" s="12">
+        <f t="shared" si="5"/>
+        <v>680641670</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
         <v>174</v>
       </c>
@@ -12394,8 +13361,20 @@
       <c r="J81" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L81" s="12">
+        <f t="shared" si="4"/>
+        <v>2.8893080462243312E+16</v>
+      </c>
+      <c r="M81" s="12">
+        <f t="shared" si="5"/>
+        <v>3.4857614782084444E+16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
         <v>203</v>
       </c>
@@ -12426,8 +13405,20 @@
       <c r="J82" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K82" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L82" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M82" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
         <v>41</v>
       </c>
@@ -12458,8 +13449,20 @@
       <c r="J83" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83" s="12">
+        <f t="shared" si="3"/>
+        <v>6869999999999313</v>
+      </c>
+      <c r="L83" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M83" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
         <v>186</v>
       </c>
@@ -12490,8 +13493,20 @@
       <c r="J84" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K84" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L84" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M84" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
         <v>221</v>
       </c>
@@ -12522,8 +13537,20 @@
       <c r="J85" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L85" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M85" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
         <v>228</v>
       </c>
@@ -12554,8 +13581,20 @@
       <c r="J86" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L86" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M86" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
         <v>82</v>
       </c>
@@ -12583,8 +13622,20 @@
       <c r="I87" s="13">
         <v>6955706069066970</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87" s="12">
+        <f t="shared" si="3"/>
+        <v>6264897854719635</v>
+      </c>
+      <c r="L87" s="12">
+        <f t="shared" si="4"/>
+        <v>29718550300</v>
+      </c>
+      <c r="M87" s="12">
+        <f t="shared" si="5"/>
+        <v>34671966310</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
         <v>223</v>
       </c>
@@ -12615,8 +13666,20 @@
       <c r="J88" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L88" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M88" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
         <v>165</v>
       </c>
@@ -12647,8 +13710,20 @@
       <c r="J89" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L89" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M89" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
         <v>172</v>
       </c>
@@ -12679,8 +13754,20 @@
       <c r="J90" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L90" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
         <v>182</v>
       </c>
@@ -12711,8 +13798,20 @@
       <c r="J91" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L91" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M91" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
         <v>177</v>
       </c>
@@ -12743,8 +13842,20 @@
       <c r="J92" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L92" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M92" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
         <v>198</v>
       </c>
@@ -12775,8 +13886,20 @@
       <c r="J93" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L93" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M93" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
         <v>139</v>
       </c>
@@ -12804,8 +13927,20 @@
       <c r="I94" s="13">
         <v>7022758435202540</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94" s="12">
+        <f t="shared" si="3"/>
+        <v>17637114064880</v>
+      </c>
+      <c r="L94" s="12">
+        <f t="shared" si="4"/>
+        <v>3596877020</v>
+      </c>
+      <c r="M94" s="12">
+        <f t="shared" si="5"/>
+        <v>3168953943069801</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
         <v>212</v>
       </c>
@@ -12836,8 +13971,20 @@
       <c r="J95" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K95" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L95" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M95" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
         <v>138</v>
       </c>
@@ -12865,8 +14012,20 @@
       <c r="I96" s="13">
         <v>7025738638553060</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96" s="12">
+        <f t="shared" si="3"/>
+        <v>20617317415400</v>
+      </c>
+      <c r="L96" s="12">
+        <f t="shared" si="4"/>
+        <v>2846756080</v>
+      </c>
+      <c r="M96" s="12">
+        <f t="shared" si="5"/>
+        <v>3168951803285901</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
         <v>219</v>
       </c>
@@ -12897,8 +14056,20 @@
       <c r="J97" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L97" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M97" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
         <v>44</v>
       </c>
@@ -12929,8 +14100,20 @@
       <c r="J98" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L98" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M98" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
         <v>136</v>
       </c>
@@ -12961,8 +14144,20 @@
       <c r="J99" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L99" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M99" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
         <v>217</v>
       </c>
@@ -12993,8 +14188,20 @@
       <c r="J100" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L100" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M100" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
         <v>218</v>
       </c>
@@ -13025,8 +14232,20 @@
       <c r="J101" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K101" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L101" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M101" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
         <v>216</v>
       </c>
@@ -13057,8 +14276,20 @@
       <c r="J102" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K102" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L102" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M102" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
         <v>224</v>
       </c>
@@ -13089,8 +14320,20 @@
       <c r="J103" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K103" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L103" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M103" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
         <v>243</v>
       </c>
@@ -13121,8 +14364,20 @@
       <c r="J104" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K104" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L104" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M104" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
         <v>240</v>
       </c>
@@ -13153,8 +14408,20 @@
       <c r="J105" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K105" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L105" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M105" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
         <v>78</v>
       </c>
@@ -13182,8 +14449,20 @@
       <c r="I106" s="12">
         <v>687.5</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K106" s="12">
+        <f t="shared" si="3"/>
+        <v>6864651989795872</v>
+      </c>
+      <c r="L106" s="12">
+        <f t="shared" si="4"/>
+        <v>3.2102926523540576E+16</v>
+      </c>
+      <c r="M106" s="12">
+        <f t="shared" si="5"/>
+        <v>3.5208812507371316E+16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
         <v>208</v>
       </c>
@@ -13214,8 +14493,20 @@
       <c r="J107" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K107" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L107" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M107" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
         <v>152</v>
       </c>
@@ -13246,8 +14537,20 @@
       <c r="J108" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K108" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L108" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M108" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
         <v>125</v>
       </c>
@@ -13278,8 +14581,20 @@
       <c r="J109" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K109" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L109" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M109" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
         <v>214</v>
       </c>
@@ -13310,8 +14625,20 @@
       <c r="J110" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K110" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L110" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M110" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
         <v>100</v>
       </c>
@@ -13339,8 +14666,20 @@
       <c r="I111" s="13">
         <v>68891098172569</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K111" s="12">
+        <f t="shared" si="3"/>
+        <v>620682150986850</v>
+      </c>
+      <c r="L111" s="12">
+        <f t="shared" si="4"/>
+        <v>2464386270</v>
+      </c>
+      <c r="M111" s="12">
+        <f t="shared" si="5"/>
+        <v>175232655</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
         <v>39</v>
       </c>
@@ -13371,8 +14710,20 @@
       <c r="J112" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K112" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L112" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M112" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
         <v>33</v>
       </c>
@@ -13400,8 +14751,20 @@
       <c r="I113" s="13">
         <v>6877614554178320</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K113" s="12">
+        <f t="shared" si="3"/>
+        <v>26610620947580</v>
+      </c>
+      <c r="L113" s="12">
+        <f t="shared" si="4"/>
+        <v>2.889429358037882E+16</v>
+      </c>
+      <c r="M113" s="12">
+        <f t="shared" si="5"/>
+        <v>43231039400</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
         <v>83</v>
       </c>
@@ -13429,8 +14792,20 @@
       <c r="I114" s="13">
         <v>6861497893587140</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K114" s="12">
+        <f t="shared" si="3"/>
+        <v>6170689679239805</v>
+      </c>
+      <c r="L114" s="12">
+        <f t="shared" si="4"/>
+        <v>2.889285723087206E+16</v>
+      </c>
+      <c r="M114" s="12">
+        <f t="shared" si="5"/>
+        <v>3168865657560489</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
         <v>67</v>
       </c>
@@ -13458,8 +14833,20 @@
       <c r="I115" s="13">
         <v>6946152531494740</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K115" s="12">
+        <f t="shared" si="3"/>
+        <v>90792594762670</v>
+      </c>
+      <c r="L115" s="12">
+        <f t="shared" si="4"/>
+        <v>2.8893204055553592E+16</v>
+      </c>
+      <c r="M115" s="12">
+        <f t="shared" si="5"/>
+        <v>3.16883348860567E+16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
         <v>231</v>
       </c>
@@ -13490,8 +14877,20 @@
       <c r="J116" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K116" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L116" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M116" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
         <v>140</v>
       </c>
@@ -13522,8 +14921,20 @@
       <c r="J117" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K117" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L117" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M117" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
         <v>91</v>
       </c>
@@ -13551,8 +14962,20 @@
       <c r="I118" s="12">
         <v>688</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K118" s="12">
+        <f t="shared" si="3"/>
+        <v>6892751431498692</v>
+      </c>
+      <c r="L118" s="12">
+        <f t="shared" si="4"/>
+        <v>3210258076151648</v>
+      </c>
+      <c r="M118" s="12">
+        <f t="shared" si="5"/>
+        <v>3.52090008742182E+16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
         <v>47</v>
       </c>
@@ -13580,8 +15003,20 @@
       <c r="I119" s="13">
         <v>6865295599244380</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K119" s="12">
+        <f t="shared" si="3"/>
+        <v>89056939383960</v>
+      </c>
+      <c r="L119" s="12">
+        <f t="shared" si="4"/>
+        <v>2889379653677368</v>
+      </c>
+      <c r="M119" s="12">
+        <f t="shared" si="5"/>
+        <v>76669025490</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
         <v>34</v>
       </c>
@@ -13612,8 +15047,20 @@
       <c r="J120" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K120" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L120" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M120" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
         <v>24</v>
       </c>
@@ -13641,8 +15088,20 @@
       <c r="I121" s="13">
         <v>6874086695278960</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K121" s="12">
+        <f t="shared" si="3"/>
+        <v>8100890145300</v>
+      </c>
+      <c r="L121" s="12">
+        <f t="shared" si="4"/>
+        <v>2889427215418822</v>
+      </c>
+      <c r="M121" s="12">
+        <f t="shared" si="5"/>
+        <v>3.168904618342508E+16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
         <v>101</v>
       </c>
@@ -13670,8 +15129,20 @@
       <c r="I122" s="12">
         <v>690</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K122" s="12">
+        <f t="shared" si="3"/>
+        <v>689573249158729</v>
+      </c>
+      <c r="L122" s="12">
+        <f t="shared" si="4"/>
+        <v>3210232722244707</v>
+      </c>
+      <c r="M122" s="12">
+        <f t="shared" si="5"/>
+        <v>352057050321441</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
         <v>49</v>
       </c>
@@ -13702,8 +15173,20 @@
       <c r="J123" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K123" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L123" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M123" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
         <v>37</v>
       </c>
@@ -13734,8 +15217,20 @@
       <c r="J124" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K124" s="12">
+        <f t="shared" si="3"/>
+        <v>6869999999999313</v>
+      </c>
+      <c r="L124" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M124" s="12">
+        <f t="shared" si="5"/>
+        <v>3.5209905839009064E+16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
         <v>19</v>
       </c>
@@ -13763,8 +15258,20 @@
       <c r="I125" s="13">
         <v>6885715257118570</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K125" s="12">
+        <f t="shared" si="3"/>
+        <v>3527671694310</v>
+      </c>
+      <c r="L125" s="12">
+        <f t="shared" si="4"/>
+        <v>2889426682751373</v>
+      </c>
+      <c r="M125" s="12">
+        <f t="shared" si="5"/>
+        <v>8961405890</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
         <v>59</v>
       </c>
@@ -13792,8 +15299,20 @@
       <c r="I126" s="12">
         <v>685</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K126" s="12">
+        <f t="shared" si="3"/>
+        <v>6898056423384105</v>
+      </c>
+      <c r="L126" s="12">
+        <f t="shared" si="4"/>
+        <v>2.8893742143850848E+16</v>
+      </c>
+      <c r="M126" s="12">
+        <f t="shared" si="5"/>
+        <v>12043203880</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
         <v>61</v>
       </c>
@@ -13824,8 +15343,20 @@
       <c r="J127" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K127" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L127" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M127" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
         <v>65</v>
       </c>
@@ -13853,8 +15384,20 @@
       <c r="I128" s="12">
         <v>685</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K128" s="12">
+        <f t="shared" si="3"/>
+        <v>6855359936731385</v>
+      </c>
+      <c r="L128" s="12">
+        <f t="shared" si="4"/>
+        <v>3.210355240775218E+16</v>
+      </c>
+      <c r="M128" s="12">
+        <f t="shared" si="5"/>
+        <v>3520887516254291</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
         <v>21</v>
       </c>
@@ -13882,8 +15425,20 @@
       <c r="I129" s="13">
         <v>686518181150371</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K129" s="12">
+        <f t="shared" si="3"/>
+        <v>6195669404273889</v>
+      </c>
+      <c r="L129" s="12">
+        <f t="shared" si="4"/>
+        <v>2889429380292335</v>
+      </c>
+      <c r="M129" s="12">
+        <f t="shared" si="5"/>
+        <v>3168909205856395</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
         <v>16</v>
       </c>
@@ -13914,8 +15469,20 @@
       <c r="J130" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K130" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L130" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M130" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
         <v>108</v>
       </c>
@@ -13946,8 +15513,20 @@
       <c r="J131" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K131" s="12">
+        <f t="shared" ref="K131:K142" si="6">ABS(E131-I131)</f>
+        <v>0</v>
+      </c>
+      <c r="L131" s="12">
+        <f t="shared" ref="L131:L142" si="7">ABS(D131-G131)</f>
+        <v>0</v>
+      </c>
+      <c r="M131" s="12">
+        <f t="shared" ref="M131:M142" si="8">ABS(C131-H131)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
         <v>134</v>
       </c>
@@ -13978,8 +15557,20 @@
       <c r="J132" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K132" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L132" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M132" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
         <v>70</v>
       </c>
@@ -14010,8 +15601,20 @@
       <c r="J133" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K133" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L133" s="12">
+        <f t="shared" si="7"/>
+        <v>3210336949588045</v>
+      </c>
+      <c r="M133" s="12">
+        <f t="shared" si="8"/>
+        <v>3520878775731248</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>159</v>
       </c>
@@ -14042,8 +15645,20 @@
       <c r="J134" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K134" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L134" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M134" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
         <v>68</v>
       </c>
@@ -14074,8 +15689,20 @@
       <c r="J135" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K135" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L135" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M135" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
         <v>93</v>
       </c>
@@ -14103,8 +15730,20 @@
       <c r="I136" s="12">
         <v>688</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K136" s="12">
+        <f t="shared" si="6"/>
+        <v>6889962870267182</v>
+      </c>
+      <c r="L136" s="12">
+        <f t="shared" si="7"/>
+        <v>3210262685085658</v>
+      </c>
+      <c r="M136" s="12">
+        <f t="shared" si="8"/>
+        <v>3520890677223591</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
         <v>73</v>
       </c>
@@ -14135,8 +15774,20 @@
       <c r="J137" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K137" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L137" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M137" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
         <v>110</v>
       </c>
@@ -14167,8 +15818,20 @@
       <c r="J138" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K138" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L138" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M138" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
         <v>56</v>
       </c>
@@ -14196,8 +15859,20 @@
       <c r="I139" s="13">
         <v>6844882369222250</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K139" s="12">
+        <f t="shared" si="6"/>
+        <v>53174054162540</v>
+      </c>
+      <c r="L139" s="12">
+        <f t="shared" si="7"/>
+        <v>10821186730</v>
+      </c>
+      <c r="M139" s="12">
+        <f t="shared" si="8"/>
+        <v>26499217580</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
         <v>95</v>
       </c>
@@ -14228,8 +15903,20 @@
       <c r="J140" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K140" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L140" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M140" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" s="10" t="s">
         <v>53</v>
       </c>
@@ -14260,8 +15947,20 @@
       <c r="J141" s="12" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K141" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L141" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M141" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" s="10" t="s">
         <v>89</v>
       </c>
@@ -14291,6 +15990,18 @@
       </c>
       <c r="J142" s="12" t="s">
         <v>268</v>
+      </c>
+      <c r="K142" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L142" s="12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M142" s="12">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>